<commit_message>
edit and add Search Criteria
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_receivable_detail.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_receivable_detail.xlsx
@@ -245,7 +245,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,6 +255,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9E2F3"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFFF"/>
         <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
@@ -306,7 +312,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -319,6 +325,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -339,7 +349,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -355,7 +365,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -439,7 +449,7 @@
   <dimension ref="A2:U20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -460,213 +470,229 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B5" s="3"/>
       <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="B8" s="3"/>
       <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="J19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="K19" s="6" t="s">
+      <c r="K19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L19" s="6" t="s">
+      <c r="L19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="M19" s="6" t="s">
+      <c r="M19" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N19" s="6" t="s">
+      <c r="N19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="O19" s="8" t="s">
+      <c r="O19" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="P19" s="8" t="s">
+      <c r="P19" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="Q19" s="8" t="s">
+      <c r="Q19" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="R19" s="8" t="s">
+      <c r="R19" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="S19" s="6" t="s">
+      <c r="S19" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="T19" s="6" t="s">
+      <c r="T19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U19" s="6" t="s">
+      <c r="U19" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10" t="s">
+      <c r="D20" s="11"/>
+      <c r="E20" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="K20" s="10" t="s">
+      <c r="K20" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="L20" s="10" t="s">
+      <c r="L20" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="M20" s="10" t="s">
+      <c r="M20" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="N20" s="10" t="s">
+      <c r="N20" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="O20" s="12" t="s">
+      <c r="O20" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="P20" s="12" t="s">
+      <c r="P20" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="Q20" s="12"/>
-      <c r="R20" s="12" t="s">
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10" t="s">
+      <c r="S20" s="11"/>
+      <c r="T20" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="U20" s="10" t="s">
+      <c r="U20" s="11" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edit and fix bug template receivable detail report excel
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_receivable_detail.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_receivable_detail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t xml:space="preserve">Receivable Detail Report</t>
   </si>
@@ -128,60 +128,6 @@
   </si>
   <si>
     <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">รหัสลูกหนี้</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ชื่อลูกหนี้</t>
-  </si>
-  <si>
-    <t xml:space="preserve">เลขที่เอกสาร</t>
-  </si>
-  <si>
-    <t xml:space="preserve">เอกสารอ้างอิง</t>
-  </si>
-  <si>
-    <t xml:space="preserve">วันที่เอกสาร</t>
-  </si>
-  <si>
-    <t xml:space="preserve">วันที่บันทึก</t>
-  </si>
-  <si>
-    <t xml:space="preserve">วันครบกำหนด</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ยอดก่อน VAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ยอด Vat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ยอดรวม</t>
-  </si>
-  <si>
-    <t xml:space="preserve">สกุลเงิน</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ภาษี</t>
-  </si>
-  <si>
-    <t xml:space="preserve">รายละเอียด</t>
-  </si>
-  <si>
-    <t xml:space="preserve">เลขที่เอกสารรับเงิน (RC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">เลขที่ใบเสร็จ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">จำนวนเงินที่จ่าย</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ผู้บันทึก KV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">สถานะ</t>
   </si>
 </sst>
 </file>
@@ -193,7 +139,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD\/MM\/YYYY"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -216,36 +162,28 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <name val="Tahoma"/>
+      <sz val="10"/>
+      <name val="arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="0"/>
+      <name val="arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10.5"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,14 +202,8 @@
         <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8EAADB"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -279,13 +211,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -312,60 +237,44 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -396,7 +305,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF8EAADB"/>
+      <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
@@ -446,254 +355,195 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:U20"/>
+  <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="13.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="13.06"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="7" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.06"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="16" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="13.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="30.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="13.06"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="7" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.06"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="16" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="21" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="D5" s="2" t="s">
+      <c r="B5" s="5"/>
+      <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="D8" s="2" t="s">
+      <c r="B7" s="5"/>
+      <c r="D7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="2" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="19" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E16" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F16" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="I16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="7" t="s">
+      <c r="J16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K19" s="7" t="s">
+      <c r="K16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="L19" s="7" t="s">
+      <c r="L16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M19" s="7" t="s">
+      <c r="M16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="N19" s="7" t="s">
+      <c r="N16" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="O19" s="9" t="s">
+      <c r="O16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="P19" s="9" t="s">
+      <c r="P16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="Q19" s="9" t="s">
+      <c r="Q16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="R19" s="9" t="s">
+      <c r="R16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="S19" s="7" t="s">
+      <c r="S16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="T19" s="7" t="s">
+      <c r="T16" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="U19" s="7" t="s">
+      <c r="U16" s="8" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="K20" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="L20" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="M20" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="N20" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="O20" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="P20" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="S20" s="11"/>
-      <c r="T20" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="U20" s="11" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix query code gl_receivable_report and Update receivable_detail_report V2 10/07/2018
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_receivable_detail.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_receivable_detail.xlsx
@@ -20,65 +20,68 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+  <si>
+    <t xml:space="preserve">Real Start Date</t>
+  </si>
   <si>
     <t xml:space="preserve">Receivable Detail Report</t>
   </si>
   <si>
+    <t xml:space="preserve">Real End Date</t>
+  </si>
+  <si>
     <t xml:space="preserve">Account Code</t>
   </si>
   <si>
+    <t xml:space="preserve">Supplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiscal Year From</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiscal Year To</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Period Length (days)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Period From</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Period To</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date From</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date To</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As of Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run By</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run Date</t>
+  </si>
+  <si>
     <t xml:space="preserve">Customer Code</t>
   </si>
   <si>
-    <t xml:space="preserve">Fiscal Year From</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fiscal Year To</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Filter by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Period From</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Period To</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date From</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date To</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Posting Date From</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Posting Date To</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document Date From</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document Date To</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document Number</t>
+    <t xml:space="preserve">Customer Name</t>
   </si>
   <si>
     <t xml:space="preserve">System Origin</t>
   </si>
   <si>
-    <t xml:space="preserve">Run By</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Run Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer Name</t>
-  </si>
-  <si>
     <t xml:space="preserve">Document Origin</t>
   </si>
   <si>
@@ -89,6 +92,12 @@
   </si>
   <si>
     <t xml:space="preserve">Due Date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Over Due (Days)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overdue Length</t>
   </si>
   <si>
     <t xml:space="preserve">Subtotal </t>
@@ -134,12 +143,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="DD\/MM\/YYYY"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="@"/>
+    <numFmt numFmtId="167" formatCode="DD\/MM\/YYYY"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -171,6 +181,13 @@
       <b val="true"/>
       <sz val="10"/>
       <name val="arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -182,8 +199,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,14 +217,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9E2F3"/>
-        <bgColor rgb="FFCCFFFF"/>
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFADD58A"/>
+        <bgColor rgb="FF99CCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FFD9E2F3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFFF"/>
-        <bgColor rgb="FFCCFFFF"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E2F3"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -237,7 +280,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -250,31 +293,55 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -294,7 +361,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -303,7 +370,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFADD58A"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -312,7 +379,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFD9E2F3"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -322,7 +389,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFD9E2F3"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
@@ -355,195 +422,234 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U16"/>
+  <dimension ref="A1:AH15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W18" activeCellId="0" sqref="W18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="13.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="30.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="13.06"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="7" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.06"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="16" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="21" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="11" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.06"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="18" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="14.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="32" min="23" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="17.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="35" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
+      <c r="AG1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5"/>
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5"/>
+      <c r="A4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="D5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="5"/>
+      <c r="A5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="0"/>
+      <c r="AG5" s="9"/>
+      <c r="AH5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5"/>
+      <c r="A6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="0"/>
+      <c r="AG6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="D7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="5"/>
+      <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="0"/>
+      <c r="AG7" s="8"/>
+      <c r="AH7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="0"/>
+      <c r="AG8" s="8"/>
+      <c r="AH8" s="10"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="0"/>
+      <c r="AG9" s="8"/>
+      <c r="AH9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="5"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="15" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="16" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="8" t="s">
+      <c r="B15" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="8" t="s">
+      <c r="D15" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="E15" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="F15" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="G15" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="H15" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="I15" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="J15" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="L16" s="8" t="s">
+      <c r="K15" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="M16" s="8" t="s">
+      <c r="L15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="N16" s="8" t="s">
+      <c r="M15" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="O16" s="8" t="s">
+      <c r="N15" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="P16" s="8" t="s">
+      <c r="O15" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="Q16" s="8" t="s">
+      <c r="P15" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="R16" s="8" t="s">
+      <c r="Q15" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="S16" s="8" t="s">
+      <c r="R15" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="T16" s="8" t="s">
+      <c r="S15" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="U16" s="8" t="s">
+      <c r="T15" s="13" t="s">
         <v>35</v>
+      </c>
+      <c r="U15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="V15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="W15" s="13" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[IMP] Adjust Receivable Detail
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_receivable_detail.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_receivable_detail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t xml:space="preserve">Real Start Date</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Account Code</t>
   </si>
   <si>
-    <t xml:space="preserve">Supplier</t>
+    <t xml:space="preserve">Customer</t>
   </si>
   <si>
     <t xml:space="preserve">Fiscal Year From</t>
@@ -67,6 +67,9 @@
     <t xml:space="preserve">Document Number</t>
   </si>
   <si>
+    <t xml:space="preserve">System Origin</t>
+  </si>
+  <si>
     <t xml:space="preserve">Run By</t>
   </si>
   <si>
@@ -77,9 +80,6 @@
   </si>
   <si>
     <t xml:space="preserve">Customer Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">System Origin</t>
   </si>
   <si>
     <t xml:space="preserve">Document Origin</t>
@@ -146,11 +146,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="@"/>
-    <numFmt numFmtId="167" formatCode="DD\/MM\/YYYY"/>
+    <numFmt numFmtId="166" formatCode="#,##0"/>
+    <numFmt numFmtId="167" formatCode="#,###.00"/>
+    <numFmt numFmtId="168" formatCode="@"/>
+    <numFmt numFmtId="169" formatCode="DD\/MM\/YYYY"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -283,17 +285,33 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -305,7 +323,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -332,7 +350,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -340,7 +358,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -425,10 +443,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AH15"/>
+  <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U4" activeCellId="0" sqref="U4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -437,225 +455,263 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="13.06"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="11" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.06"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="18" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="32" min="24" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="19.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="17.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="35" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="25.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="21.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="22.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="21.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="23.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="22.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="4" width="23.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="28.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="23.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="32" min="25" style="5" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="5" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="5" width="17.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="35" style="5" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2"/>
-      <c r="AG1" s="3" t="s">
+    <row r="1" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6"/>
+      <c r="AG1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="AH1" s="4"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="AH1" s="8"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AG2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AH2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="AH2" s="8"/>
+      <c r="AMJ2" s="0"/>
+    </row>
+    <row r="3" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="AG3" s="8"/>
-      <c r="AH3" s="8"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="AG3" s="12"/>
+      <c r="AH3" s="12"/>
+      <c r="AMJ3" s="0"/>
+    </row>
+    <row r="4" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="AG4" s="8"/>
-      <c r="AH4" s="8"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="AG4" s="12"/>
+      <c r="AH4" s="12"/>
+      <c r="AMJ4" s="0"/>
+    </row>
+    <row r="5" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="11"/>
       <c r="E5" s="0"/>
-      <c r="AG5" s="9"/>
-      <c r="AH5" s="8"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="AG5" s="13"/>
+      <c r="AH5" s="12"/>
+      <c r="AMJ5" s="0"/>
+    </row>
+    <row r="6" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="8"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="0"/>
-      <c r="AG6" s="3" t="s">
+      <c r="AG6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="AH6" s="10"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="AH6" s="14"/>
+      <c r="AMJ6" s="0"/>
+    </row>
+    <row r="7" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="0"/>
-      <c r="AG7" s="8"/>
-      <c r="AH7" s="10"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="AG7" s="12"/>
+      <c r="AH7" s="14"/>
+      <c r="AMJ7" s="0"/>
+    </row>
+    <row r="8" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="11"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="0"/>
-      <c r="AG8" s="8"/>
-      <c r="AH8" s="10"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="AG8" s="12"/>
+      <c r="AH8" s="14"/>
+      <c r="AMJ8" s="0"/>
+    </row>
+    <row r="9" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="8"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="12"/>
       <c r="E9" s="0"/>
-      <c r="AG9" s="8"/>
-      <c r="AH9" s="10"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="AG9" s="12"/>
+      <c r="AH9" s="14"/>
+      <c r="AMJ9" s="0"/>
+    </row>
+    <row r="10" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="8"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="12"/>
       <c r="E10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
+      <c r="AMJ10" s="0"/>
+    </row>
+    <row r="11" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
       <c r="E11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+      <c r="AMJ11" s="0"/>
+    </row>
+    <row r="12" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="0"/>
+      <c r="AMJ12" s="0"/>
+    </row>
+    <row r="13" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="15" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="AMJ13" s="0"/>
+    </row>
+    <row r="14" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="AMJ14" s="0"/>
+    </row>
+    <row r="15" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMJ15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="B16" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="13" t="s">
+      <c r="D16" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F16" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G16" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H16" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="I16" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="15" t="s">
+      <c r="J16" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="K15" s="13" t="s">
+      <c r="K16" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="L15" s="13" t="s">
+      <c r="L16" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="M15" s="13" t="s">
+      <c r="M16" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="N15" s="13" t="s">
+      <c r="N16" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="O15" s="13" t="s">
+      <c r="O16" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="P15" s="13" t="s">
+      <c r="P16" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="Q15" s="13" t="s">
+      <c r="Q16" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="R15" s="13" t="s">
+      <c r="R16" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="S15" s="13" t="s">
+      <c r="S16" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="T15" s="13" t="s">
+      <c r="T16" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="U15" s="13" t="s">
+      <c r="U16" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="V15" s="13" t="s">
+      <c r="V16" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="W15" s="13" t="s">
+      <c r="W16" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="X15" s="13" t="s">
+      <c r="X16" s="17" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>